<commit_message>
Added scroll_and_load() to get more data from google map page. Added Colorma to print colored info.
</commit_message>
<xml_diff>
--- a/展覽設計公司.xlsx
+++ b/展覽設計公司.xlsx
@@ -1,31 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c94c6e6290610b5a/desktop/Git_Repositories/ExhibitionDesignCompaniesSearching/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_5D75C0E8F613C8A64DB3FB1469CA909471ACFE1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{157B388B-B081-466D-AD2A-296D8BDE7071}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="109">
   <si>
     <t>公司名稱</t>
   </si>
   <si>
-    <t>網址</t>
+    <t>網站</t>
+  </si>
+  <si>
+    <t>Google評分</t>
   </si>
   <si>
     <t>地址</t>
@@ -34,150 +31,327 @@
     <t>電話</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>王一設計</t>
-  </si>
-  <si>
-    <t>米瑞克</t>
-  </si>
-  <si>
-    <t>olily.com</t>
-  </si>
-  <si>
-    <t>Viva Design 欣豐設計</t>
-  </si>
-  <si>
-    <t>PRO360</t>
-  </si>
-  <si>
-    <t>艾爾克</t>
-  </si>
-  <si>
-    <t>o-ya-design.com</t>
-  </si>
-  <si>
-    <t>104人力銀行</t>
-  </si>
-  <si>
-    <t>興隨興展覽股份有限公司</t>
-  </si>
-  <si>
-    <t>輝祐展覽設計</t>
+    <t>雅得展覽設計</t>
+  </si>
+  <si>
+    <t>米瑞克展覽設計有限公司</t>
+  </si>
+  <si>
+    <t>立大展設計</t>
+  </si>
+  <si>
+    <t>艾爾克展覽設計</t>
+  </si>
+  <si>
+    <t>VIVA DESIGN欣豐設計有限公司</t>
+  </si>
+  <si>
+    <t>奧森展覽設計 Ocean Expo Design.Co.,Ltd</t>
+  </si>
+  <si>
+    <t>王一設計 KingOne Design</t>
+  </si>
+  <si>
+    <t>元墉國際/展覽設計/快閃店/公關活動/室內設計/店面商業空間裝修</t>
+  </si>
+  <si>
+    <t>京典展覽設計有限公司</t>
+  </si>
+  <si>
+    <t>藝創國際空間設計有限公司</t>
+  </si>
+  <si>
+    <t>尚展空間設計有限公司</t>
+  </si>
+  <si>
+    <t>愷奕國際展覽設計有限公司</t>
+  </si>
+  <si>
+    <t>格式｜設計展策 InFormat Design Curating</t>
+  </si>
+  <si>
+    <t>悅馳展覽設計有限公司</t>
+  </si>
+  <si>
+    <t>展躍有限公司 - RiseCreatives 展躍網路</t>
+  </si>
+  <si>
+    <t>歐立利國際展覽設計 OLILY │展覽設計│展場設計│攤位設計</t>
+  </si>
+  <si>
+    <t>大於展覽設計有限公司</t>
+  </si>
+  <si>
+    <t>靠設計廣告｜展覽策劃｜展覽佈置｜AR擴增實境｜VR虛擬實境｜實境行銷｜活動策劃｜活動佈置｜廣告物設計｜道具製作｜大圖輸出</t>
+  </si>
+  <si>
+    <t>【U-Design 環球創意】公關策劃 | 活動規劃 | 視覺創意 | 展覽設計 | 硬體整合</t>
+  </si>
+  <si>
+    <t>宏展國際 中山（展覽設計 硬體租貸）</t>
+  </si>
+  <si>
+    <t>祈邑設計有限公司</t>
+  </si>
+  <si>
+    <t>奧茲品牌策展有限公司</t>
+  </si>
+  <si>
+    <t>黎京國際設計有限公司</t>
+  </si>
+  <si>
+    <t>歐也空間室內裝修設計股份有限公司</t>
+  </si>
+  <si>
+    <t>卡邦國際空間設計有限公司</t>
+  </si>
+  <si>
+    <t>https://www.yade.com.tw/</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>https://echodesignn.com/</t>
+  </si>
+  <si>
+    <t>http://www.vivadesign.com.tw/</t>
+  </si>
+  <si>
+    <t>https://oceandesign.com.tw/</t>
   </si>
   <si>
     <t>https://www.kingone-design.com/</t>
   </si>
   <si>
-    <t>http://www.mymiracleart.com/</t>
-  </si>
-  <si>
-    <t>https://www.olily.com/project.html</t>
-  </si>
-  <si>
-    <t>https://www.vivadesign.com.tw/</t>
-  </si>
-  <si>
-    <t>https://www.pro360.com.tw/category/exhibition_design</t>
-  </si>
-  <si>
-    <t>https://echodesignn.com/exhibition-category</t>
-  </si>
-  <si>
-    <t>https://www.o-ya-design.com/</t>
-  </si>
-  <si>
-    <t>https://www.104.com.tw/company/search/?keyword=%E5%B1%95%E8%A6%BD%E8%A8%AD%E8%A8%88</t>
-  </si>
-  <si>
-    <t>https://www.thetwdesign.com/</t>
-  </si>
-  <si>
-    <t>https://www.hydesign.com.tw/</t>
-  </si>
-  <si>
-    <t>[('百大上市', '', '', '', '', '', '', ''), ('9個城市', '', '', '', '', '', '', ''), ('智慧城市', '', '', '', '', '', '', ''), ('海內外市', '', '', '', '', '', '', ''), (' 台北市', '松山區', '復興北路', '', '', '167號', '12樓之2', '')]</t>
-  </si>
-  <si>
-    <t>[('\n台北市', '松山區', '八德路', '', '', '', '', '')]</t>
-  </si>
-  <si>
-    <t>[('獅爺門市', '', '', '', '', '', '', ''), ('\n台北市', '南港區', '三重路', '', '', '', '', '')]</t>
-  </si>
-  <si>
-    <t>[(' 新北市', '中和區', '中正路', '', '', '916號', '8樓', '')]</t>
-  </si>
-  <si>
-    <t>[('\n新竹市', '', '', '', '', '', '', ''), ('\n台中市', '北屯區', '', '', '', '', '', ''), ('\n台北市', '南港區', '', '', '', '', '', ''), ('\n台北市', '信義區', '', '', '', '', '', '')]</t>
-  </si>
-  <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>[('\n台北市', '南港區', '三重路', '', '', '', '', '')]</t>
-  </si>
-  <si>
-    <t>[('\n新北市', '汐止區', '', '', '', '', '', ''), ('司\n上市', '', '', '', '', '', '', ''), ('\n台北市', '中山區', '', '', '', '', '', ''), ('\n台北市', '松山區', '', '', '', '', '', ''), ('◆臺北市', '', '', '', '', '', '', ''), ('於台中市', '', '', '', '', '', '', ''), ('是台中市', '', '', '', '', '', '', ''), ('\n 上市', '', '', '', '', '', '', ''), ('虛擬城市', '', '', '', '', '', '', ''), ('\n台北市', '信義區', '', '', '', '', '', ''), ('內外上市', '', '', '', '', '', '', ''), ('\n台北市', '南港區', '', '', '', '', '', ''), ('主要城市', '', '', '', '', '', '', ''), ('於台北市', '信義區', '', '', '', '', '', ''), ('\n台北市', '大同區', '', '', '', '', '', ''), ('，集合市', '', '', '', '', '', '', ''), ('\n台中市', '烏日區', '', '', '', '', '', ''), ('\n台中市', '西屯區', '', '', '', '', '', ''), ('家具備市', '', '', '', '', '', '', ''), ('中\n上市', '', '', '', '', '', '', ''), ('如台中市', '', '', '', '', '', '', '')]</t>
-  </si>
-  <si>
-    <t>[('主要城市', '', '', '', '', '', '', ''), ('\n桃園市', '', '', '', '', '', '', ''), (' 金門縣', '文化園區', '', '', '', '', '', ''), ('重要城市', '', '', '', '', '', '', ''), ('淨零城市', '', '', '', '', '', '', '')]</t>
-  </si>
-  <si>
-    <t>[(' 台北市', '信義區', '信義路', '', '', '', '', '')]</t>
-  </si>
-  <si>
-    <t>[('20', ''), ('19', ''), ('1932', ''), ('2010', ''), ('9083', ''), ('17', ''), ('23', ''), ('8083', ''), ('150', ''), ('21', ''), ('105403', ''), ('550', ''), ('886-2-2718', ''), ('360', ''), ('2023', ''), ('12', ''), ('15', ''), ('2024', ''), ('2022', ''), ('167', ''), ('24', '')]</t>
-  </si>
-  <si>
-    <t>[('26', ''), ('2023-01-06', ''), ('2023-05-30', ''), ('09', ''), ('30-18', ''), ('2023-06-28', ''), ('2023', ''), ('2018', ''), ('123', ''), ('886', ''), ('30', ''), ('(02)2760-0576', '02'), ('(02)2760-0057', '02'), ('2023-01-19', '')]</t>
-  </si>
-  <si>
-    <t>[('720', ''), ('19', ''), ('886-2-2655', ''), ('10', ''), ('1989', ''), ('20121', ''), ('100', ''), ('101', ''), ('2021', '')]</t>
-  </si>
-  <si>
-    <t>[('50', ''), ('40', ''), ('0999', '09'), ('916', ''), ('01', ''), ('886-2-2226', ''), ('02-2226-0091', '02'), ('886-2-2221', ''), ('0928853992', '09288'), ('235015', ''), ('0289', '02'), ('11', ''), ('886-2-2223', ''), ('02', ''), ('2017', ''), ('3-7', ''), ('8089', '')]</t>
-  </si>
-  <si>
-    <t>[('2019-12-13', ''), ('2019', ''), ('20', ''), ('700', ''), ('10', ''), ('35-40', ''), ('5-7', ''), ('200', ''), ('2022-10-14', ''), ('13', ''), ('2023-11-06', ''), ('2019-05-27', ''), ('90378737', ''), ('2023-06-16', ''), ('10-20', ''), ('285', ''), ('2022-08-16', ''), ('2022-04-01', ''), ('2020-03-20', ''), ('360', ''), ('2019-05-17', ''), ('30', ''), ('2024', ''), ('100', ''), ('2021-08-31', ''), ('372', ''), ('36', ''), ('2022-01-05', ''), ('2000', ''), ('25', ''), ('108', ''), ('00', ''), ('2018-04-27', ''), ('22', ''), ('580', ''), ('110', ''), ('2024-02-01', '')]</t>
-  </si>
-  <si>
-    <t>[('2006-2024', ''), ('25', ''), ('380', ''), ('220', ''), ('10', ''), ('5-2', ''), ('500', ''), ('12', ''), ('11', ''), ('15', ''), ('2-3', ''), ('110', ''), ('24', '')]</t>
-  </si>
-  <si>
-    <t>[('720', ''), ('19', ''), ('2024-06-19', ''), ('160', ''), ('130', ''), ('(02)2655-2777', '02'), ('10', ''), ('360', ''), ('2023', ''), ('2050', ''), ('2024-06-14', ''), ('2024', ''), ('22', ''), ('110', ''), ('2024-06-07', ''), ('2021', ''), ('4088', '')]</t>
-  </si>
-  <si>
-    <t>[('1\n2\n3', ''), ('20', ''), ('19', ''), ('09', ''), ('01', ''), ('04', ''), ('111', ''), ('185', ''), ('1951', ''), ('10', ''), ('700', ''), ('31', ''), ('600', ''), ('500', ''), ('4\n5', ''), ('17', ''), ('03', ''), ('43', ''), ('05', ''), ('2017', ''), ('06', ''), ('23', ''), ('13', ''), ('26', ''), ('42', ''), ('4488', ''), ('2014', ''), ('35', ''), ('14', ''), ('32', ''), ('29', ''), ('38', ''), ('2295', ''), ('11', ''), ('02', ''), ('81', ''), ('33', ''), ('800', ''), ('21', ''), ('1990', ''), ('34', ''), ('40', ''), ('39', ''), ('140', ''), ('1981', ''), ('37', ''), ('12', ''), ('27', ''), ('97', ''), ('506', ''), ('15', ''), ('30', ''), ('1988', ''), ('80', ''), ('2024', ''), ('1993', ''), ('36', ''), ('2022', ''), ('07', ''), ('16', ''), ('2000', ''), ('25', ''), ('41', ''), ('1994', ''), ('18', ''), ('104', ''), ('08', ''), ('76', ''), ('2016', ''), ('50-100', ''), ('22', ''), ('24', ''), ('28', '')]</t>
-  </si>
-  <si>
-    <t>[('20', ''), ('2020-12-15', ''), ('2021-11-12', ''), ('2022-04-29', ''), ('1997', ''), ('2022-01-21', ''), ('2024-03-29', ''), ('2024-05-09', ''), ('2015', ''), ('2021-04-21', ''), ('2024-05-16', ''), ('2024-01-01', ''), ('2022-04-27', ''), ('2023', ''), ('2024-01-04', ''), ('2024', ''), ('2022', ''), ('2022-05-26', ''), ('2022-04-22', ''), ('2050', ''), ('2021', ''), ('2023-12-06', '')]</t>
-  </si>
-  <si>
-    <t>[('1\n2\n3', ''), ('09', ''), ('10', ''), ('4\n5', ''), ('17', ''), ('43', ''), ('35', ''), ('1986', ''), ('2021-12-15', ''), ('02 8789 8300', '02'), ('2020', ''), ('2023', ''), ('2022', ''), ('02 2729 7976', '02'), ('2020-06-11', ''), ('18', ''), ('00', ''), ('20121', ''), ('110', ''), ('2021', '')]</t>
-  </si>
-  <si>
-    <t>['info@kingone-design.com']</t>
-  </si>
-  <si>
-    <t>['service@mymiracleart.com']</t>
-  </si>
-  <si>
-    <t>['mkt02@vivadesign.com.tw', 'mkt01@vivadesign.com.tw']</t>
-  </si>
-  <si>
-    <t>['ina@ms17.hinet.net']</t>
+    <t>http://yuan-yong.com/</t>
+  </si>
+  <si>
+    <t>http://classic-ds.com.tw/</t>
+  </si>
+  <si>
+    <t>http://www.ultraxdesign.com/</t>
+  </si>
+  <si>
+    <t>https://www.simpleinterior.com.tw/</t>
+  </si>
+  <si>
+    <t>http://informat-design.com.tw/</t>
+  </si>
+  <si>
+    <t>https://www.yes168.com.tw/</t>
+  </si>
+  <si>
+    <t>https://www.raise-up.com.tw/</t>
+  </si>
+  <si>
+    <t>https://www.olily.com/</t>
+  </si>
+  <si>
+    <t>https://ud168.com/</t>
+  </si>
+  <si>
+    <t>https://www.home-show.com.tw/</t>
+  </si>
+  <si>
+    <t>http://www.ozzie-art.com/</t>
+  </si>
+  <si>
+    <t>https://www.designspace-expo.com/</t>
+  </si>
+  <si>
+    <t>http://www.o-ya-design.com/</t>
+  </si>
+  <si>
+    <t>http://www.cp-design.com.tw/</t>
+  </si>
+  <si>
+    <t>5.0</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>no comments</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>4.9</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>南京東路五段188號6號樓之5</t>
+  </si>
+  <si>
+    <t>八德路四段123號7樓</t>
+  </si>
+  <si>
+    <t>中山北路二段189巷15弄12號1樓</t>
+  </si>
+  <si>
+    <t>碧華街416號4樓</t>
+  </si>
+  <si>
+    <t>中正路916號8樓</t>
+  </si>
+  <si>
+    <t>龍江路147號2F</t>
+  </si>
+  <si>
+    <t>復興北路167號12樓之2</t>
+  </si>
+  <si>
+    <t>辛亥路四段77巷52號B1</t>
+  </si>
+  <si>
+    <t>基隆路一段155號</t>
+  </si>
+  <si>
+    <t>忠孝東路四段276號12樓</t>
+  </si>
+  <si>
+    <t>光復南路417號7樓</t>
+  </si>
+  <si>
+    <t>設計公司</t>
+  </si>
+  <si>
+    <t>龍江路415巷20號</t>
+  </si>
+  <si>
+    <t>中山路74號</t>
+  </si>
+  <si>
+    <t>復興南路二段293之3號5樓之2</t>
+  </si>
+  <si>
+    <t>三重路19-6號10樓</t>
+  </si>
+  <si>
+    <t>3樓,No.36號松德路</t>
+  </si>
+  <si>
+    <t>西寧北路78號9樓912室</t>
+  </si>
+  <si>
+    <t>新北大道三段5號13F之6</t>
+  </si>
+  <si>
+    <t>合江街31巷14號B1</t>
+  </si>
+  <si>
+    <t>宏國路51號</t>
+  </si>
+  <si>
+    <t>玉門街1號</t>
+  </si>
+  <si>
+    <t>115東新街130號1樓</t>
+  </si>
+  <si>
+    <t>南京東路六段461號9號樓之1</t>
+  </si>
+  <si>
+    <t>02 2947 9452</t>
+  </si>
+  <si>
+    <t>02 2760 0057</t>
+  </si>
+  <si>
+    <t>0930 616 729</t>
+  </si>
+  <si>
+    <t>02 2857 8831</t>
+  </si>
+  <si>
+    <t>02 2226 0999</t>
+  </si>
+  <si>
+    <t>02 2369 0999</t>
+  </si>
+  <si>
+    <t>02 2718 8083</t>
+  </si>
+  <si>
+    <t>02 2523 9976</t>
+  </si>
+  <si>
+    <t>02 2759 2899</t>
+  </si>
+  <si>
+    <t>02 8771 9698</t>
+  </si>
+  <si>
+    <t>02 2720 8568</t>
+  </si>
+  <si>
+    <t>02 7730 2967</t>
+  </si>
+  <si>
+    <t>02 2518 5905</t>
+  </si>
+  <si>
+    <t>02 7703 0655</t>
+  </si>
+  <si>
+    <t>02 7741 7454</t>
+  </si>
+  <si>
+    <t>02 2655 1989</t>
+  </si>
+  <si>
+    <t>02 8786 0303</t>
+  </si>
+  <si>
+    <t>0978 511 151</t>
+  </si>
+  <si>
+    <t>02 8522 7599</t>
+  </si>
+  <si>
+    <t>04 2426 0965</t>
+  </si>
+  <si>
+    <t>02 2729 7122</t>
+  </si>
+  <si>
+    <t>02 2788 9008</t>
+  </si>
+  <si>
+    <t>02 2655 2777</t>
+  </si>
+  <si>
+    <t>02 2795 1119</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -185,7 +359,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -195,13 +369,6 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="新細明體"/>
-      <family val="3"/>
-      <charset val="136"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -251,26 +418,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -308,7 +467,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -342,7 +501,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -377,10 +535,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -553,21 +710,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="29.0703125" customWidth="1"/>
-    <col min="2" max="2" width="74.640625" customWidth="1"/>
-    <col min="3" max="3" width="56.5" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" customWidth="1"/>
-    <col min="5" max="5" width="51.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,189 +734,452 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
+      <c r="B3" t="s">
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
+      <c r="B4" t="s">
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="B21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+      <c r="E25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>54</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" t="s">
+        <v>108</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="B11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B10" r:id="rId7"/>
+    <hyperlink ref="B11" r:id="rId8"/>
+    <hyperlink ref="B12" r:id="rId9"/>
+    <hyperlink ref="B14" r:id="rId10"/>
+    <hyperlink ref="B15" r:id="rId11"/>
+    <hyperlink ref="B16" r:id="rId12"/>
+    <hyperlink ref="B17" r:id="rId13"/>
+    <hyperlink ref="B20" r:id="rId14"/>
+    <hyperlink ref="B21" r:id="rId15"/>
+    <hyperlink ref="B23" r:id="rId16"/>
+    <hyperlink ref="B24" r:id="rId17"/>
+    <hyperlink ref="B25" r:id="rId18"/>
+    <hyperlink ref="B26" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>